<commit_message>
Documentation applied for the functions created. Also, student names in th Excel file modified.
</commit_message>
<xml_diff>
--- a/students_scores.xlsx
+++ b/students_scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twist\OneDrive\Documentos\Desarrollos\Python\Word_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F3F469-3C03-4CA8-8481-6E2D31BCFC54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1464B56-186C-4680-B1B6-57C53D8754C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Nombre</t>
   </si>
@@ -96,6 +96,36 @@
   </si>
   <si>
     <t>juan.reyes@web.com</t>
+  </si>
+  <si>
+    <t>Gael Barroso</t>
+  </si>
+  <si>
+    <t>Maria Ines Vargas</t>
+  </si>
+  <si>
+    <t>Enriqueta Pérez</t>
+  </si>
+  <si>
+    <t>Carmelo Gascon</t>
+  </si>
+  <si>
+    <t>Ian Lago</t>
+  </si>
+  <si>
+    <t>Fatiha Agullo</t>
+  </si>
+  <si>
+    <t>Cristina Maria Prados</t>
+  </si>
+  <si>
+    <t>Jairo Vila</t>
+  </si>
+  <si>
+    <t>Maria Alicia Roca</t>
+  </si>
+  <si>
+    <t>Hipolito Montiel</t>
   </si>
 </sst>
 </file>
@@ -131,9 +161,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,7 +475,7 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>21</v>
       </c>
       <c r="C2" t="s">
@@ -460,7 +489,7 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>22</v>
       </c>
       <c r="C3" t="s">
@@ -653,7 +682,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -677,7 +706,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -691,7 +720,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>9</v>
@@ -705,7 +734,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -719,7 +748,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B5">
         <v>9</v>
@@ -733,7 +762,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>7</v>
@@ -747,7 +776,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -761,7 +790,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -775,7 +804,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B9">
         <v>10</v>
@@ -789,7 +818,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -803,7 +832,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B11">
         <v>8</v>

</xml_diff>

<commit_message>
Function to send email with the grades created. Missing attaching file to the email
</commit_message>
<xml_diff>
--- a/students_scores.xlsx
+++ b/students_scores.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twist\OneDrive\Documentos\Desarrollos\Python\Word_Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Development\Python\WordAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1464B56-186C-4680-B1B6-57C53D8754C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Maestro" sheetId="1" r:id="rId1"/>
     <sheet name="Matematicas" sheetId="2" r:id="rId2"/>
     <sheet name="Desarrollo Web" sheetId="3" r:id="rId3"/>
+    <sheet name="samples" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>Nombre</t>
   </si>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -161,8 +161,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,22 +443,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -485,7 +486,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -505,19 +506,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{444557B0-7752-46D6-A1BA-E2F1C082E1CE}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19:G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -531,7 +532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -545,7 +546,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -559,117 +560,9 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>9</v>
-      </c>
-      <c r="D8">
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9">
-        <v>10</v>
-      </c>
-      <c r="C9">
-        <v>10</v>
-      </c>
-      <c r="D9">
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11">
-        <v>8</v>
-      </c>
-      <c r="C11">
-        <v>6</v>
-      </c>
-      <c r="D11">
-        <v>9.9</v>
-      </c>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -678,19 +571,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0091ED8E-7D92-418C-B0FB-2A2E0186AA9C}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -704,7 +597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -718,7 +611,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -732,7 +625,100 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>9</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>9.6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -745,8 +731,20 @@
       <c r="D4">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>9</v>
+      </c>
+      <c r="I4">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -759,8 +757,20 @@
       <c r="D5">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -773,8 +783,20 @@
       <c r="D6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="H6">
+        <v>7</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -787,8 +809,20 @@
       <c r="D7">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -801,8 +835,20 @@
       <c r="D8">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>9</v>
+      </c>
+      <c r="I8">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -815,8 +861,20 @@
       <c r="D9">
         <v>8.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -829,8 +887,20 @@
       <c r="D10">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -841,6 +911,18 @@
         <v>6</v>
       </c>
       <c r="D11">
+        <v>9.9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
+      <c r="H11">
+        <v>6</v>
+      </c>
+      <c r="I11">
         <v>9.9</v>
       </c>
     </row>

</xml_diff>